<commit_message>
Added dataset "res1C_focus_hand" to data-raw/
</commit_message>
<xml_diff>
--- a/data-raw/res1A_focus_hand.xlsx
+++ b/data-raw/res1A_focus_hand.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zurp/Dropbox (Personal)/diss/analy/vid-coding/hand-focus-res-1-A. done/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zurp/Dropbox (Personal)/diss/analy/vid-coding/res1A-focus-hand. done/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="mdg-20171117" sheetId="1" r:id="rId1"/>
-    <sheet name="slg-20171117" sheetId="3" r:id="rId2"/>
+    <sheet name="mdg_20171117" sheetId="1" r:id="rId1"/>
+    <sheet name="slg_20171117" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -1363,7 +1363,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>